<commit_message>
update excel format table
</commit_message>
<xml_diff>
--- a/Cahier des charges/UserStory.xlsx
+++ b/Cahier des charges/UserStory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feder\Documents\AR-U-Here\Cahier des charges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6015FA-14B1-4DC9-A42A-37340404D35D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BDE9D91-01F6-4ED0-B7BD-8CE8494162C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -290,8 +290,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A5:F50" totalsRowShown="0">
   <autoFilter ref="A5:F50" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A33:F46">
-    <sortCondition ref="D5:D49"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:F50">
+    <sortCondition ref="D5:D50"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Objet"/>
@@ -301,7 +301,7 @@
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="personne en charge"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Importance"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -604,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1188,19 +1188,19 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="B33" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C33">
         <v>4</v>
       </c>
       <c r="D33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E33" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="F33" t="s">
         <v>52</v>
@@ -1208,10 +1208,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B34" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C34">
         <v>4</v>
@@ -1220,7 +1220,7 @@
         <v>3</v>
       </c>
       <c r="E34" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F34" t="s">
         <v>52</v>
@@ -1228,19 +1228,19 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B35" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C35">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D35">
         <v>3</v>
       </c>
       <c r="E35" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F35" t="s">
         <v>52</v>
@@ -1248,10 +1248,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C36">
         <v>2</v>
@@ -1262,13 +1262,10 @@
       <c r="E36" t="s">
         <v>13</v>
       </c>
-      <c r="F36" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B37" t="s">
         <v>7</v>
@@ -1280,29 +1277,32 @@
         <v>3</v>
       </c>
       <c r="E37" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="B38" t="s">
         <v>7</v>
       </c>
       <c r="C38">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D38">
         <v>3</v>
       </c>
       <c r="E38" t="s">
-        <v>8</v>
+        <v>28</v>
+      </c>
+      <c r="F38" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B39" t="s">
         <v>7</v>
@@ -1322,10 +1322,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B40" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C40">
         <v>4</v>
@@ -1334,7 +1334,7 @@
         <v>3</v>
       </c>
       <c r="E40" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="F40" t="s">
         <v>52</v>
@@ -1342,33 +1342,33 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B41" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="C41">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D41">
         <v>3</v>
       </c>
       <c r="E41" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F41" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B42" t="s">
         <v>38</v>
       </c>
       <c r="C42">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D42">
         <v>3</v>
@@ -1377,15 +1377,15 @@
         <v>9</v>
       </c>
       <c r="F42" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B43" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="C43">
         <v>4</v>
@@ -1402,33 +1402,33 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B44" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C44">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D44">
         <v>3</v>
       </c>
       <c r="E44" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="F44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>58</v>
+      <c r="A45" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="B45" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C45">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D45">
         <v>3</v>
@@ -1437,12 +1437,12 @@
         <v>28</v>
       </c>
       <c r="F45" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
-        <v>59</v>
+      <c r="A46" t="s">
+        <v>61</v>
       </c>
       <c r="B46" t="s">
         <v>24</v>
@@ -1454,7 +1454,7 @@
         <v>3</v>
       </c>
       <c r="E46" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F46" t="s">
         <v>52</v>
@@ -1462,50 +1462,50 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="B47" t="s">
         <v>11</v>
       </c>
       <c r="C47">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D47">
         <v>4</v>
       </c>
       <c r="E47" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="F47" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B48" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C48">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D48">
         <v>4</v>
       </c>
       <c r="E48" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B49" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C49">
         <v>4</v>
@@ -1514,7 +1514,7 @@
         <v>4</v>
       </c>
       <c r="E49" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F49" t="s">
         <v>52</v>
@@ -1522,7 +1522,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="B50" t="s">
         <v>24</v>
@@ -1531,10 +1531,10 @@
         <v>4</v>
       </c>
       <c r="D50">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E50" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F50" t="s">
         <v>52</v>

</xml_diff>